<commit_message>
Sprint Burndownchart eingefügt und Autorinformationen angepasst
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6570" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="SprintBurndownchart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Nr</t>
   </si>
@@ -144,6 +145,18 @@
   </si>
   <si>
     <t>StoryID</t>
+  </si>
+  <si>
+    <t>Summe der Points</t>
+  </si>
+  <si>
+    <t>Tage</t>
+  </si>
+  <si>
+    <t>StoryPoints</t>
+  </si>
+  <si>
+    <t>Diagonale</t>
   </si>
 </sst>
 </file>
@@ -173,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -181,18 +194,145 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -213,10 +353,278 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SprintBurndownchart!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StoryPoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>SprintBurndownchart!$A$4:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SprintBurndownchart!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diagonale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>SprintBurndownchart!$C$4:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="106844928"/>
+        <c:axId val="106846464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="106844928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="106846464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="106846464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="106844928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81421151248099599"/>
+          <c:y val="0.4422110598244185"/>
+          <c:w val="0.18578839925711041"/>
+          <c:h val="0.13856638609828945"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -254,9 +662,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,7 +699,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +734,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -502,17 +910,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="98.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -520,7 +928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -537,7 +945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -554,7 +962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>21</v>
       </c>
@@ -562,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>22</v>
       </c>
@@ -570,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>23</v>
       </c>
@@ -578,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>24</v>
       </c>
@@ -586,7 +994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>25</v>
       </c>
@@ -594,7 +1002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>26</v>
       </c>
@@ -602,7 +1010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -619,7 +1027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>31</v>
       </c>
@@ -627,7 +1035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>32</v>
       </c>
@@ -635,7 +1043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -652,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>51</v>
       </c>
@@ -660,7 +1068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>52</v>
       </c>
@@ -668,7 +1076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>53</v>
       </c>
@@ -676,7 +1084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -693,7 +1101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>41</v>
       </c>
@@ -701,7 +1109,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>42</v>
       </c>
@@ -709,7 +1117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>43</v>
       </c>
@@ -717,7 +1125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>44</v>
       </c>
@@ -725,7 +1133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>45</v>
       </c>
@@ -733,7 +1141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -750,7 +1158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>11</v>
       </c>
@@ -758,7 +1166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>12</v>
       </c>
@@ -766,7 +1174,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>13</v>
       </c>
@@ -781,19 +1189,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -812,8 +1221,11 @@
       <c r="F1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -828,8 +1240,12 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <f>SUM(C2:C25)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21</v>
       </c>
@@ -851,7 +1267,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22</v>
       </c>
@@ -873,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23</v>
       </c>
@@ -895,7 +1311,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24</v>
       </c>
@@ -917,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -939,7 +1355,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>26</v>
       </c>
@@ -961,7 +1377,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>30</v>
       </c>
@@ -977,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31</v>
       </c>
@@ -999,7 +1415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32</v>
       </c>
@@ -1021,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
@@ -1037,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>51</v>
       </c>
@@ -1059,7 +1475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>52</v>
       </c>
@@ -1081,7 +1497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>53</v>
       </c>
@@ -1103,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>40</v>
       </c>
@@ -1119,7 +1535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41</v>
       </c>
@@ -1141,7 +1557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -1163,7 +1579,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43</v>
       </c>
@@ -1185,7 +1601,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>44</v>
       </c>
@@ -1207,7 +1623,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>45</v>
       </c>
@@ -1229,7 +1645,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1245,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1267,7 +1683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1289,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1311,7 +1727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" t="e">
         <f>VLOOKUP(A26,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1321,7 +1737,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" t="e">
         <f>VLOOKUP(A27,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1331,7 +1747,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" t="e">
         <f>VLOOKUP(A28,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1341,7 +1757,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" t="e">
         <f>VLOOKUP(A29,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1351,7 +1767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" t="e">
         <f>VLOOKUP(A30,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1361,7 +1777,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" t="e">
         <f>VLOOKUP(A31,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1371,7 +1787,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" t="e">
         <f>VLOOKUP(A32,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1381,7 +1797,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="e">
         <f>VLOOKUP(A33,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1391,7 +1807,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="e">
         <f>VLOOKUP(A34,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1401,7 +1817,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="e">
         <f>VLOOKUP(A35,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1411,7 +1827,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="e">
         <f>VLOOKUP(A36,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1421,7 +1837,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="e">
         <f>VLOOKUP(A37,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1431,7 +1847,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="e">
         <f>VLOOKUP(A38,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1441,7 +1857,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="e">
         <f>VLOOKUP(A39,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1451,7 +1867,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="e">
         <f>VLOOKUP(A40,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1461,7 +1877,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="e">
         <f>VLOOKUP(A41,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1471,7 +1887,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="e">
         <f>VLOOKUP(A42,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1481,7 +1897,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="e">
         <f>VLOOKUP(A43,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1491,7 +1907,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="e">
         <f>VLOOKUP(A44,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1501,7 +1917,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="e">
         <f>VLOOKUP(A45,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1511,7 +1927,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="e">
         <f>VLOOKUP(A46,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1521,7 +1937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="e">
         <f>VLOOKUP(A47,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1531,7 +1947,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="e">
         <f>VLOOKUP(A48,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1541,7 +1957,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="e">
         <f>VLOOKUP(A49,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1551,7 +1967,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="e">
         <f>VLOOKUP(A50,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1561,7 +1977,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="e">
         <f>VLOOKUP(A51,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1571,7 +1987,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="e">
         <f>VLOOKUP(A52,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1581,7 +1997,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="e">
         <f>VLOOKUP(A53,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1591,7 +2007,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="e">
         <f>VLOOKUP(A54,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1601,7 +2017,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="e">
         <f>VLOOKUP(A55,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1611,7 +2027,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="e">
         <f>VLOOKUP(A56,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1621,7 +2037,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="e">
         <f>VLOOKUP(A57,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1631,7 +2047,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="e">
         <f>VLOOKUP(A58,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1641,7 +2057,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="e">
         <f>VLOOKUP(A59,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1651,7 +2067,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" t="e">
         <f>VLOOKUP(A60,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1661,7 +2077,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" t="e">
         <f>VLOOKUP(A61,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1671,7 +2087,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" t="e">
         <f>VLOOKUP(A62,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1681,7 +2097,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" t="e">
         <f>VLOOKUP(A63,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1691,7 +2107,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" t="e">
         <f>VLOOKUP(A64,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1701,7 +2117,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" t="e">
         <f>VLOOKUP(A65,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1711,7 +2127,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="e">
         <f>VLOOKUP(A66,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1721,7 +2137,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="e">
         <f>VLOOKUP(A67,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1731,7 +2147,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="e">
         <f>VLOOKUP(A68,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1741,7 +2157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" t="e">
         <f>VLOOKUP(A69,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1751,7 +2167,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" t="e">
         <f>VLOOKUP(A70,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1761,7 +2177,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" t="e">
         <f>VLOOKUP(A71,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1771,7 +2187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" t="e">
         <f>VLOOKUP(A72,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1781,7 +2197,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" t="e">
         <f>VLOOKUP(A73,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1791,7 +2207,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" t="e">
         <f>VLOOKUP(A74,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1801,7 +2217,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" t="e">
         <f>VLOOKUP(A75,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1811,7 +2227,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" t="e">
         <f>VLOOKUP(A76,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1821,7 +2237,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" t="e">
         <f>VLOOKUP(A77,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1831,7 +2247,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" t="e">
         <f>VLOOKUP(A78,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1841,7 +2257,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" t="e">
         <f>VLOOKUP(A79,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1851,7 +2267,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B80" t="e">
         <f>VLOOKUP(A80,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1861,7 +2277,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" t="e">
         <f>VLOOKUP(A81,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1871,7 +2287,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" t="e">
         <f>VLOOKUP(A82,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1881,7 +2297,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" t="e">
         <f>VLOOKUP(A83,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1891,7 +2307,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" t="e">
         <f>VLOOKUP(A84,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1901,7 +2317,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" t="e">
         <f>VLOOKUP(A85,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1911,7 +2327,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" t="e">
         <f>VLOOKUP(A86,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1921,7 +2337,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" t="e">
         <f>VLOOKUP(A87,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1931,7 +2347,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" t="e">
         <f>VLOOKUP(A88,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1941,7 +2357,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" t="e">
         <f>VLOOKUP(A89,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1951,7 +2367,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" t="e">
         <f>VLOOKUP(A90,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1961,7 +2377,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" t="e">
         <f>VLOOKUP(A91,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1974,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" t="e">
         <f>VLOOKUP(A92,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1987,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" t="e">
         <f>VLOOKUP(A93,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1997,7 +2413,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" t="e">
         <f>VLOOKUP(A94,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -2007,7 +2423,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" t="e">
         <f>VLOOKUP(A95,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -2017,7 +2433,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" t="e">
         <f>VLOOKUP(A96,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -2027,37 +2443,308 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" t="e">
         <f>VLOOKUP(A97,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" t="e">
         <f>VLOOKUP(A98,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" t="e">
         <f>VLOOKUP(A99,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" t="e">
         <f>VLOOKUP(A100,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A1:F1048576 H1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>Tabelle2!H2</f>
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>A4</f>
+        <v>34</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>-2*B5+34</f>
+        <v>32</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C17" si="0">-2*B6+34</f>
+        <v>30</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <f>A18</f>
+        <v>8</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Login Änderung DAtenbank und Sprint eingefügt!
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6576" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6576" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="SprintBurndownchart" sheetId="3" r:id="rId3"/>
+    <sheet name="ProduktBacklog" sheetId="4" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
+    <sheet name="SprintBurndownchart" sheetId="3" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>Nr</t>
   </si>
@@ -157,6 +162,126 @@
   </si>
   <si>
     <t>Diagonale</t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich Urlaubsanträge einsehen können</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich auch über meinen Browser, meine Arbeitsstunden einsehen können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Mitarbeiter möchte ich auch über meinen Browser, Urlaubsanträge stellen können. </t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich einen Arbeitsplan erstellen/ändern können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenbankschema erstellen für den Dienstplan </t>
+  </si>
+  <si>
+    <t>SWT realisieren der Oberfläche</t>
+  </si>
+  <si>
+    <t>Alvin</t>
+  </si>
+  <si>
+    <t>Nachrichten DatenBank</t>
+  </si>
+  <si>
+    <t>Nachrichten PHP (Kommentarfeld)</t>
+  </si>
+  <si>
+    <t>Tabelle für PHP</t>
+  </si>
+  <si>
+    <t>2.Sprint</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich mich über mein Android smartphone einloggen</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Userstory</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Geschäftsleiter möchte ich an meinem Arbeitsplatz die Arbeitsstunden und damit verbundene Daten abrufen können. </t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich eine Tagesübersicht über den aktuellen Dienstplan haben.</t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich Veränderungsnachweise (Historie) anzeigen lassen.</t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich eine Auswertung der gearbeiteten Stunden pro Tag der jeweiligen MA haben.</t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich eine Statistik über die gearbeiteten Wochenenden erstellen lassen.</t>
+  </si>
+  <si>
+    <t>Als Administrator möchte ich einfach von meinem Arbeitsplatz aus, Berechtigungen erteilen können.</t>
+  </si>
+  <si>
+    <t>Als Administrator möchte ich eine Liste aller Mitarbeiter und Anwender in der auch Rechte vergeben werden können.</t>
+  </si>
+  <si>
+    <t>Als Administrator möchte ich Zugriff auf sämtliche Tools und Anwendungen die benutzt werden können.</t>
+  </si>
+  <si>
+    <t>Als Administrator möchte ich eine Stelle für Feedbacks von Anwendern und zum Erkennen von Wartungs- und Verbesserungsarbeiten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Administrator möchte ich Einträge die Anwender gemacht haben ändern können. </t>
+  </si>
+  <si>
+    <t>Als Administrator möchte ich Reports erhalten, wann und von wem Einträge gemacht wurden.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich auch mit meinem Android Smartphone Urlaubsanträge stellen können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Mitarbeiter möchte ich auch mit meinem Android Smartphone meine Arbeitsstunden einsehen können </t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich Kontakt zu anderen Mitarbeitern aufnehmen können.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich über einen Tausch der Mitarbeiter benachrichtigt werden bzw. eine Bestätigung abschicken.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich einen Überblick der monatlichen Stunden erstellen können.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich mit den einzelnen Mitarbeiter kommunizieren können.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich Zugriff auf die Stammdaten der Mitarbeiter haben.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich jeden Mitarbeiter nach Namen suchen.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich eine Frist setzen können, in der die MA ihre nicht möglichen Arbeitstage eintragen.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich eie freien Tage/Urlaub der MA eintragen können.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich einen Dienstplan generieren lassen.</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter der Personalabteilung möchte ich Oberflächen mit swt haben</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich Kommetar hinterlassen</t>
   </si>
 </sst>
 </file>
@@ -309,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -321,11 +446,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -354,6 +547,323 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Product</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Burndown Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.4803149606299227E-2"/>
+          <c:y val="0.14393518518518519"/>
+          <c:w val="0.89019685039370078"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>[2]Tabelle1!$B$35:$B$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[2]Tabelle1!$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>[2]Tabelle1!$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="71513216"/>
+        <c:axId val="71540736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="71513216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71540736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71540736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71513216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="94000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -523,11 +1033,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106844928"/>
-        <c:axId val="106846464"/>
+        <c:axId val="109144704"/>
+        <c:axId val="109150592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106844928"/>
+        <c:axId val="109144704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +1046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106846464"/>
+        <c:crossAx val="109150592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -544,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106846464"/>
+        <c:axId val="109150592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,7 +1065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106844928"/>
+        <c:crossAx val="109144704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -590,6 +1100,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -619,6 +1166,287 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+      <sheetName val="Tabelle2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1">
+        <row r="1">
+          <cell r="E1" t="str">
+            <v>1. Sprint</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Nr</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>Bezeichnung</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Story-Points</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>Rang</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>20</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Als Personalleiter möchte ich mich einloggen können</v>
+          </cell>
+          <cell r="D3">
+            <v>8</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>I</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>21</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>ERM</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>22</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>DB Tabelle erstellen</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>23</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>Java Login GUI</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>24</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>Java Login Code</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>25</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>Java DB Anbindung</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>26</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>MD5 Verschlüsselung</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>30</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>Als Mitarbeiter der Personalabteilung möchte ich neue Mitarbeiter anlegen können</v>
+          </cell>
+          <cell r="D10">
+            <v>8</v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>II</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>31</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>Java GUI</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>32</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>Java Insert Code</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>50</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>Als Mitarbeiter der Personalabteilung  möchte ich Mitarbeiter suchen können</v>
+          </cell>
+          <cell r="D13">
+            <v>5</v>
+          </cell>
+          <cell r="E13" t="str">
+            <v>III</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>51</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>Java GUI</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>52</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>Java Select Code</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>53</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>Mitarbeiter nach Suche selektierbar machen</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>40</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>Als Mitarbeiter der Personalabteilung möchte ich Mitarbeiter verwalten (ändern + löschen) können</v>
+          </cell>
+          <cell r="D17">
+            <v>8</v>
+          </cell>
+          <cell r="E17" t="str">
+            <v>IV</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>41</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>Java GUI</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>42</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>Java Mitarbeiter Select Code</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>43</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>Update</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>44</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>Delete</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>45</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>Rückmeldung</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>10</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>Als Mitarbeiter möchte ich mich einloggen können</v>
+          </cell>
+          <cell r="D23">
+            <v>5</v>
+          </cell>
+          <cell r="E23" t="str">
+            <v>V</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>11</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>PHP DB Anbindung</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>12</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>PHP Oberfläche</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>13</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>PHP Funktion Login</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="8">
+          <cell r="E8">
+            <v>34</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35">
+            <v>320</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -908,10 +1736,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="117" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="13" t="str">
+        <f>VLOOKUP(B2,[1]Tabelle1!B:F,2,0)</f>
+        <v>Als Mitarbeiter möchte ich mich einloggen können</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f>VLOOKUP(B3,[1]Tabelle1!B:F,2,0)</f>
+        <v>Als Personalleiter möchte ich mich einloggen können</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="13" t="str">
+        <f>VLOOKUP(B4,[1]Tabelle1!B:F,2,0)</f>
+        <v>Als Mitarbeiter der Personalabteilung möchte ich neue Mitarbeiter anlegen können</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="13" t="str">
+        <f>VLOOKUP(B5,[1]Tabelle1!B:F,2,0)</f>
+        <v>Als Mitarbeiter der Personalabteilung möchte ich Mitarbeiter verwalten (ändern + löschen) können</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="13" t="str">
+        <f>VLOOKUP(B6,[1]Tabelle1!B:F,2,0)</f>
+        <v>Als Mitarbeiter der Personalabteilung  möchte ich Mitarbeiter suchen können</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <f>E2+E3+E4+E5+E6</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>70</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>310</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>120</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>130</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>140</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>160</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>170</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>180</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>190</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>200</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>340</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>210</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>220</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>230</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>240</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>250</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>260</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>270</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>280</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>290</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>330</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>300</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>320</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>"MOD($A2:$A,10)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>"MOD($A2:$A,10)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>"MOD($A2:$A,10)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>"MOD($A2:$A,10)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>"MOD($A2:$A,10)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,17 +2405,133 @@
         <v>31</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>310</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>311</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>200</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>310</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>220</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>320</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>330</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>340</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>341</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>342</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41</v>
       </c>
@@ -1557,7 +2896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -1579,7 +2918,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43</v>
       </c>
@@ -1601,7 +2940,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>44</v>
       </c>
@@ -1623,7 +2962,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>45</v>
       </c>
@@ -1645,7 +2984,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1661,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1683,7 +3022,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1705,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1727,97 +3066,155 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" t="e">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>310</v>
+      </c>
+      <c r="B26" t="str">
         <f>VLOOKUP(A26,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C26" t="e">
+        <v>Als Mitarbeiter möchte ich auch über meinen Browser, meine Arbeitsstunden einsehen können.</v>
+      </c>
+      <c r="C26">
         <f>VLOOKUP(A26,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" t="e">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26">
+        <f>SUM(C26:C34)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>311</v>
+      </c>
+      <c r="B27" t="str">
         <f>VLOOKUP(A27,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C27" t="e">
+        <v xml:space="preserve">Datenbankschema erstellen für den Dienstplan </v>
+      </c>
+      <c r="C27">
         <f>VLOOKUP(A27,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="e">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="B28" t="str">
         <f>VLOOKUP(A28,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C28" t="e">
+        <v xml:space="preserve">Als Mitarbeiter möchte ich auch über meinen Browser, Urlaubsanträge stellen können. </v>
+      </c>
+      <c r="C28">
         <f>VLOOKUP(A28,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" t="e">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>220</v>
+      </c>
+      <c r="B29" t="str">
         <f>VLOOKUP(A29,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C29" t="e">
+        <v>Als Mitarbeiter der Personalabteilung möchte ich einen Arbeitsplan erstellen/ändern können.</v>
+      </c>
+      <c r="C29">
         <f>VLOOKUP(A29,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" t="e">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>320</v>
+      </c>
+      <c r="B30" t="str">
         <f>VLOOKUP(A30,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C30" t="e">
+        <v>Als Mitarbeiter möchte ich mich über mein Android smartphone einloggen</v>
+      </c>
+      <c r="C30">
         <f>VLOOKUP(A30,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" t="e">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>330</v>
+      </c>
+      <c r="B31" t="str">
         <f>VLOOKUP(A31,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C31" t="e">
+        <v>SWT realisieren der Oberfläche</v>
+      </c>
+      <c r="C31">
         <f>VLOOKUP(A31,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" t="e">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>340</v>
+      </c>
+      <c r="B32" t="str">
         <f>VLOOKUP(A32,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C32" t="e">
+        <v>Nachrichten DatenBank</v>
+      </c>
+      <c r="C32">
         <f>VLOOKUP(A32,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="e">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>341</v>
+      </c>
+      <c r="B33" t="str">
         <f>VLOOKUP(A33,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C33" t="e">
+        <v>Nachrichten PHP (Kommentarfeld)</v>
+      </c>
+      <c r="C33">
         <f>VLOOKUP(A33,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" t="e">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>342</v>
+      </c>
+      <c r="B34" t="str">
         <f>VLOOKUP(A34,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C34" t="e">
+        <v>Tabelle für PHP</v>
+      </c>
+      <c r="C34">
         <f>VLOOKUP(A34,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="e">
         <f>VLOOKUP(A35,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1827,7 +3224,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="e">
         <f>VLOOKUP(A36,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1837,7 +3234,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="e">
         <f>VLOOKUP(A37,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1847,7 +3244,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="e">
         <f>VLOOKUP(A38,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1857,7 +3254,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="e">
         <f>VLOOKUP(A39,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1867,7 +3264,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="e">
         <f>VLOOKUP(A40,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1877,7 +3274,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="e">
         <f>VLOOKUP(A41,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1887,7 +3284,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="e">
         <f>VLOOKUP(A42,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1897,7 +3294,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="e">
         <f>VLOOKUP(A43,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1907,7 +3304,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="e">
         <f>VLOOKUP(A44,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1917,7 +3314,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="e">
         <f>VLOOKUP(A45,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1927,7 +3324,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" t="e">
         <f>VLOOKUP(A46,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1937,7 +3334,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="e">
         <f>VLOOKUP(A47,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -1947,7 +3344,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" t="e">
         <f>VLOOKUP(A48,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -2376,6 +3773,9 @@
         <f>VLOOKUP(A90,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" t="e">
@@ -2399,9 +3799,6 @@
         <f>VLOOKUP(A92,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E92">
-        <v>1</v>
-      </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" t="e">
@@ -2434,10 +3831,6 @@
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" t="e">
-        <f>VLOOKUP(A96,Tabelle1!B:F,2,0)</f>
-        <v>#N/A</v>
-      </c>
       <c r="C96" t="e">
         <f>VLOOKUP(A96,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
@@ -2461,15 +3854,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C100" t="e">
-        <f>VLOOKUP(A100,Tabelle1!B:F,3,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:F1048576 H1">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="H1 A1:F1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2478,12 +3865,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
User story geändert + Stunden eingetragen
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6576" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProduktBacklog" sheetId="4" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t xml:space="preserve">Datenbankschema erstellen für den Dienstplan </t>
   </si>
   <si>
-    <t>SWT realisieren der Oberfläche</t>
-  </si>
-  <si>
     <t>Alvin</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Als Mitarbeiter möchte ich Kommetar hinterlassen</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich mich auf einer SWT-Oberfläche einloggen, Daten hinzufügen, ändern und löschen können</t>
   </si>
 </sst>
 </file>
@@ -455,42 +455,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -549,7 +514,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -702,11 +667,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="71513216"/>
-        <c:axId val="71540736"/>
+        <c:axId val="88499328"/>
+        <c:axId val="88500864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71513216"/>
+        <c:axId val="88499328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,10 +710,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71540736"/>
+        <c:crossAx val="88500864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71540736"/>
+        <c:axId val="88500864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -805,10 +770,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71513216"/>
+        <c:crossAx val="88499328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -852,7 +817,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -866,7 +831,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1033,11 +998,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109144704"/>
-        <c:axId val="109150592"/>
+        <c:axId val="88530304"/>
+        <c:axId val="95048832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109144704"/>
+        <c:axId val="88530304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109150592"/>
+        <c:crossAx val="95048832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1054,7 +1019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109150592"/>
+        <c:axId val="95048832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109144704"/>
+        <c:crossAx val="88530304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1738,30 +1703,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="117" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1779,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1797,7 +1762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1815,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1833,7 +1798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1851,53 +1816,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E7">
         <f>E2+E3+E4+E5+E6</f>
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>70</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>80</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>90</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>100</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1908,71 +1873,71 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>110</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>120</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>130</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>140</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>150</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>160</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>170</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>180</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1983,7 +1948,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1994,23 +1959,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>340</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>210</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>220</v>
       </c>
@@ -2018,84 +1983,84 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>230</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>240</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>250</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>260</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>270</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>280</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>290</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>330</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>300</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>320</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2133,17 +2098,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="98.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2151,7 +2116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2168,7 +2133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2185,7 +2150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>21</v>
       </c>
@@ -2193,7 +2158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>22</v>
       </c>
@@ -2201,7 +2166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>23</v>
       </c>
@@ -2209,7 +2174,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>24</v>
       </c>
@@ -2217,7 +2182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>25</v>
       </c>
@@ -2225,7 +2190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>26</v>
       </c>
@@ -2233,7 +2198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2250,7 +2215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>31</v>
       </c>
@@ -2258,7 +2223,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>32</v>
       </c>
@@ -2266,7 +2231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2283,7 +2248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>51</v>
       </c>
@@ -2291,7 +2256,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>52</v>
       </c>
@@ -2299,7 +2264,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>53</v>
       </c>
@@ -2307,7 +2272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2324,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>41</v>
       </c>
@@ -2332,7 +2297,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>42</v>
       </c>
@@ -2340,7 +2305,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>43</v>
       </c>
@@ -2348,7 +2313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>44</v>
       </c>
@@ -2356,7 +2321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>45</v>
       </c>
@@ -2364,7 +2329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2381,7 +2346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>11</v>
       </c>
@@ -2389,7 +2354,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>12</v>
       </c>
@@ -2397,7 +2362,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>13</v>
       </c>
@@ -2405,12 +2370,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>310</v>
       </c>
@@ -2421,7 +2386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>311</v>
       </c>
@@ -2432,7 +2397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>200</v>
       </c>
@@ -2443,7 +2408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>310</v>
       </c>
@@ -2454,7 +2419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>220</v>
       </c>
@@ -2465,56 +2430,56 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>320</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>330</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="D35">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>340</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>341</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>342</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38">
         <v>13</v>
@@ -2530,18 +2495,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.85546875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2564,7 +2529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -2584,7 +2549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21</v>
       </c>
@@ -2606,7 +2571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22</v>
       </c>
@@ -2628,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23</v>
       </c>
@@ -2650,7 +2615,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24</v>
       </c>
@@ -2672,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -2694,7 +2659,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>26</v>
       </c>
@@ -2716,7 +2681,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>30</v>
       </c>
@@ -2732,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31</v>
       </c>
@@ -2754,7 +2719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32</v>
       </c>
@@ -2776,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
@@ -2792,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>51</v>
       </c>
@@ -2814,7 +2779,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>52</v>
       </c>
@@ -2836,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>53</v>
       </c>
@@ -2858,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>40</v>
       </c>
@@ -2874,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>41</v>
       </c>
@@ -2896,7 +2861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -2918,7 +2883,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43</v>
       </c>
@@ -2940,7 +2905,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>44</v>
       </c>
@@ -2962,7 +2927,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>45</v>
       </c>
@@ -2984,7 +2949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -3000,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
@@ -3022,7 +2987,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -3044,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>13</v>
       </c>
@@ -3066,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>310</v>
       </c>
@@ -3086,7 +3051,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>311</v>
       </c>
@@ -3102,7 +3067,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>200</v>
       </c>
@@ -3118,7 +3083,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>220</v>
       </c>
@@ -3131,10 +3096,10 @@
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>320</v>
       </c>
@@ -3150,23 +3115,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>330</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(A31,Tabelle1!B:F,2,0)</f>
-        <v>SWT realisieren der Oberfläche</v>
+        <v>Als Mitarbeiter möchte ich mich auf einer SWT-Oberfläche einloggen, Daten hinzufügen, ändern und löschen können</v>
       </c>
       <c r="C31">
         <f>VLOOKUP(A31,Tabelle1!B:F,3,0)</f>
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>340</v>
       </c>
@@ -3182,7 +3153,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>341</v>
       </c>
@@ -3198,7 +3169,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>342</v>
       </c>
@@ -3214,7 +3185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" t="e">
         <f>VLOOKUP(A35,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3224,7 +3195,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" t="e">
         <f>VLOOKUP(A36,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3234,7 +3205,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" t="e">
         <f>VLOOKUP(A37,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3244,7 +3215,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" t="e">
         <f>VLOOKUP(A38,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3254,7 +3225,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" t="e">
         <f>VLOOKUP(A39,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3264,7 +3235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="e">
         <f>VLOOKUP(A40,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3274,7 +3245,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="e">
         <f>VLOOKUP(A41,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3284,7 +3255,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="e">
         <f>VLOOKUP(A42,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3294,7 +3265,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="e">
         <f>VLOOKUP(A43,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3304,7 +3275,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="e">
         <f>VLOOKUP(A44,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3314,7 +3285,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="e">
         <f>VLOOKUP(A45,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3324,7 +3295,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="e">
         <f>VLOOKUP(A46,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3334,7 +3305,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="e">
         <f>VLOOKUP(A47,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3344,7 +3315,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="e">
         <f>VLOOKUP(A48,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3354,7 +3325,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="e">
         <f>VLOOKUP(A49,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3364,7 +3335,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="e">
         <f>VLOOKUP(A50,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3374,7 +3345,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="e">
         <f>VLOOKUP(A51,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3384,7 +3355,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="e">
         <f>VLOOKUP(A52,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3394,7 +3365,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="e">
         <f>VLOOKUP(A53,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3404,7 +3375,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="e">
         <f>VLOOKUP(A54,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3414,7 +3385,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="e">
         <f>VLOOKUP(A55,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3424,7 +3395,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="e">
         <f>VLOOKUP(A56,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3434,7 +3405,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="e">
         <f>VLOOKUP(A57,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3444,7 +3415,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="e">
         <f>VLOOKUP(A58,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3454,7 +3425,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="e">
         <f>VLOOKUP(A59,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3464,7 +3435,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="e">
         <f>VLOOKUP(A60,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3474,7 +3445,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="e">
         <f>VLOOKUP(A61,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3484,7 +3455,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="e">
         <f>VLOOKUP(A62,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3494,7 +3465,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="e">
         <f>VLOOKUP(A63,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3504,7 +3475,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="e">
         <f>VLOOKUP(A64,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3514,7 +3485,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="e">
         <f>VLOOKUP(A65,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3524,7 +3495,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="e">
         <f>VLOOKUP(A66,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3534,7 +3505,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="e">
         <f>VLOOKUP(A67,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3544,7 +3515,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="e">
         <f>VLOOKUP(A68,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3554,7 +3525,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="e">
         <f>VLOOKUP(A69,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3564,7 +3535,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="e">
         <f>VLOOKUP(A70,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3574,7 +3545,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="e">
         <f>VLOOKUP(A71,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3584,7 +3555,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="e">
         <f>VLOOKUP(A72,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3594,7 +3565,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="e">
         <f>VLOOKUP(A73,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3604,7 +3575,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="e">
         <f>VLOOKUP(A74,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3614,7 +3585,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="e">
         <f>VLOOKUP(A75,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3624,7 +3595,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="e">
         <f>VLOOKUP(A76,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3634,7 +3605,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="e">
         <f>VLOOKUP(A77,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3644,7 +3615,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="e">
         <f>VLOOKUP(A78,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3654,7 +3625,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="e">
         <f>VLOOKUP(A79,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3664,7 +3635,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="e">
         <f>VLOOKUP(A80,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3674,7 +3645,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="e">
         <f>VLOOKUP(A81,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3684,7 +3655,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="e">
         <f>VLOOKUP(A82,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3694,7 +3665,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" t="e">
         <f>VLOOKUP(A83,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3704,7 +3675,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" t="e">
         <f>VLOOKUP(A84,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3714,7 +3685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" t="e">
         <f>VLOOKUP(A85,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3724,7 +3695,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" t="e">
         <f>VLOOKUP(A86,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3734,7 +3705,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" t="e">
         <f>VLOOKUP(A87,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3744,7 +3715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" t="e">
         <f>VLOOKUP(A88,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3754,7 +3725,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" t="e">
         <f>VLOOKUP(A89,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3764,7 +3735,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" t="e">
         <f>VLOOKUP(A90,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3777,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" t="e">
         <f>VLOOKUP(A91,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3790,7 +3761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" t="e">
         <f>VLOOKUP(A92,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3800,7 +3771,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" t="e">
         <f>VLOOKUP(A93,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3810,7 +3781,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" t="e">
         <f>VLOOKUP(A94,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3820,7 +3791,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" t="e">
         <f>VLOOKUP(A95,Tabelle1!B:F,2,0)</f>
         <v>#N/A</v>
@@ -3830,25 +3801,25 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C96" t="e">
         <f>VLOOKUP(A96,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" t="e">
         <f>VLOOKUP(A97,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" t="e">
         <f>VLOOKUP(A98,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" t="e">
         <f>VLOOKUP(A99,Tabelle1!B:F,3,0)</f>
         <v>#N/A</v>
@@ -3873,11 +3844,11 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>